<commit_message>
add todojob dans labview + update OT
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/OT_.Default - Copie.xlsx
+++ b/lib/PHPExcel/templates/OT_.Default - Copie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18795" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18795" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSTT FR" sheetId="1" r:id="rId1"/>
@@ -242,12 +242,6 @@
     <font>
       <sz val="8"/>
       <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -294,6 +288,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -304,7 +304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor rgb="FFA6B4A8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,27 +381,27 @@
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -410,7 +410,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -425,7 +425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,7 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -443,22 +443,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -569,22 +569,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>456479</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
+        <xdr:cNvPr id="5" name="Image 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E18AD1-7A85-434C-B348-8B9DBE5388DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F65FF3-DD48-4459-998F-22044B93713F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -593,71 +593,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6467476" y="0"/>
-          <a:ext cx="476250" cy="2238375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>233362</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF990B9C-4D48-4384-BB5D-67A4AD941258}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6581776" y="0"/>
-          <a:ext cx="476250" cy="2476500"/>
+          <a:off x="6581775" y="314325"/>
+          <a:ext cx="475529" cy="2200275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -748,22 +692,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>451716</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
+        <xdr:cNvPr id="6" name="Image 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A02B8A95-6ACC-4248-803A-8DBF0DBEC62E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1171DDB7-ED4D-4110-904B-4C27C25B770A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -772,21 +716,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6581776" y="0"/>
-          <a:ext cx="476250" cy="2481263"/>
+          <a:off x="6577012" y="314325"/>
+          <a:ext cx="475529" cy="2200275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1344,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1597,8 +1535,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>